<commit_message>
update template qpp021 A
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_A.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_A.xlsx
@@ -18,13 +18,9 @@
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -62,13 +58,6 @@
       <family val="3"/>
       <charset val="128"/>
     </font>
-    <font>
-      <sz val="8"/>
-      <color theme="1"/>
-      <name val="IPA明朝"/>
-      <family val="1"/>
-      <charset val="128"/>
-    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -79,12 +68,12 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="5">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -133,21 +122,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </left>
-      <right style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </right>
-      <top style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </top>
-      <bottom style="thin">
-        <color theme="1" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -161,27 +135,28 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="4" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -467,10 +442,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="22.5" customHeight="1"/>
@@ -484,24 +459,27 @@
     <row r="1" spans="1:9" ht="22.5" customHeight="1">
       <c r="F1" s="4"/>
       <c r="G1" s="4"/>
-      <c r="H1" s="6"/>
-      <c r="I1" s="6"/>
+      <c r="H1" s="3"/>
+      <c r="I1" s="3"/>
     </row>
     <row r="2" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="2"/>
+      <c r="A2" s="1"/>
+      <c r="B2" s="1"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="6"/>
     </row>
     <row r="3" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A3" s="3"/>
-      <c r="B3" s="3"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="2"/>
+      <c r="A3" s="1"/>
+      <c r="B3" s="1"/>
+      <c r="C3" s="5"/>
+      <c r="D3" s="6"/>
     </row>
     <row r="5" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A5" s="5"/>
-      <c r="B5" s="7"/>
+      <c r="A5" s="2"/>
+      <c r="B5" s="8"/>
+    </row>
+    <row r="12" spans="1:9" ht="22.5" customHeight="1">
+      <c r="C12" s="7"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>

<commit_message>
update service impl jpa
</commit_message>
<xml_diff>
--- a/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_A.xlsx
+++ b/nts.uk/file/pr/nts.uk.file.pr.infra/src/main/resources/report/QPP021_A.xlsx
@@ -4,12 +4,13 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr filterPrivacy="1"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22230" windowHeight="6450"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="125725"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -20,7 +21,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -31,13 +32,6 @@
     <font>
       <u/>
       <sz val="15"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="20"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -57,6 +51,30 @@
       <name val="Meiryo UI"/>
       <family val="3"/>
       <charset val="128"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="22"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="25"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="16"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="3">
@@ -68,7 +86,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -125,39 +143,41 @@
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0">
+    <xf numFmtId="38" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="38" fontId="4" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" textRotation="255" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="255"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -442,50 +462,90 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.42578125" defaultRowHeight="22.5" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="18.28515625" customWidth="1"/>
-    <col min="2" max="2" width="22.140625" customWidth="1"/>
-    <col min="3" max="3" width="20.42578125" customWidth="1"/>
-    <col min="4" max="4" width="20.28515625" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" customWidth="1"/>
+    <col min="3" max="3" width="8.5703125" customWidth="1"/>
+    <col min="4" max="4" width="10.140625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+    <col min="6" max="6" width="9.7109375" customWidth="1"/>
+    <col min="7" max="7" width="11" customWidth="1"/>
+    <col min="8" max="8" width="10.28515625" customWidth="1"/>
+    <col min="9" max="9" width="10.42578125" customWidth="1"/>
+    <col min="10" max="10" width="9.42578125" customWidth="1"/>
+    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="12" max="12" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="10.140625" customWidth="1"/>
+    <col min="14" max="14" width="9.5703125" customWidth="1"/>
+    <col min="15" max="16" width="9.42578125" customWidth="1"/>
+    <col min="17" max="17" width="11.42578125" customWidth="1"/>
+    <col min="18" max="18" width="11.28515625" customWidth="1"/>
+    <col min="19" max="19" width="10.5703125" customWidth="1"/>
+    <col min="20" max="20" width="10.28515625" customWidth="1"/>
+    <col min="21" max="21" width="11.28515625" customWidth="1"/>
+    <col min="22" max="22" width="9.85546875" customWidth="1"/>
+    <col min="23" max="23" width="12.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="22.5" customHeight="1">
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
+    <row r="1" spans="1:12" ht="39.75" customHeight="1">
+      <c r="F1" s="2"/>
+      <c r="G1" s="3"/>
       <c r="H1" s="3"/>
-      <c r="I1" s="3"/>
+      <c r="I1" s="4"/>
+      <c r="J1" s="4"/>
+      <c r="K1" s="4"/>
+      <c r="L1" s="4"/>
     </row>
-    <row r="2" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="5"/>
-      <c r="D2" s="6"/>
+    <row r="2" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A2" s="8"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="7"/>
+      <c r="D2" s="7"/>
+      <c r="E2" s="7"/>
+      <c r="F2" s="7"/>
+      <c r="G2" s="7"/>
+      <c r="H2" s="7"/>
     </row>
-    <row r="3" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="6"/>
+    <row r="3" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A3" s="8"/>
+      <c r="B3" s="9"/>
+      <c r="C3" s="7"/>
+      <c r="D3" s="7"/>
+      <c r="E3" s="7"/>
+      <c r="F3" s="7"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
     </row>
-    <row r="5" spans="1:9" ht="22.5" customHeight="1">
-      <c r="A5" s="2"/>
-      <c r="B5" s="8"/>
+    <row r="5" spans="1:12" ht="22.5" customHeight="1">
+      <c r="A5" s="10"/>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
     </row>
-    <row r="12" spans="1:9" ht="22.5" customHeight="1">
-      <c r="C12" s="7"/>
+    <row r="6" spans="1:12" ht="22.5" customHeight="1">
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+    </row>
+    <row r="12" spans="1:12" ht="22.5" customHeight="1">
+      <c r="C12" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="3">
-    <mergeCell ref="F1:G1"/>
+  <mergeCells count="9">
+    <mergeCell ref="I1:L1"/>
+    <mergeCell ref="B5:C5"/>
+    <mergeCell ref="B6:C6"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="C3:D3"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="E3:H3"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="61" orientation="landscape" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>